<commit_message>
Added basic math classes and foreign language classes
</commit_message>
<xml_diff>
--- a/Course Description Sample Sheet.xlsx
+++ b/Course Description Sample Sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1568630\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1326952\Desktop\Poole-Shedoole\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="160">
   <si>
     <t>English 9</t>
   </si>
@@ -459,6 +459,51 @@
   </si>
   <si>
     <t>(sample) study hall</t>
+  </si>
+  <si>
+    <t>Students develop the ability to communicate about Personal and Family Life, School Life, Social Life, and Community Life using simple sentences containing basic language structure. This course counts towards the world languages course for the Advanced Studies Diploma.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students learn to function in real-life situations using more complex language structures and a wider range of vocabulary. Explore themes of Home Life, Student Life, Leisure Time, and Vacation and Travel. </t>
+  </si>
+  <si>
+    <t>Students will learn to use simple sentence structures and basic language structures to discuss about Personal and Family Life, School Life, Social Life, and Community Life. They will develop their listening, speaking, reading, and writing skills.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students continue to develop their skills in listening, speaking, reading, and writing, while learning how to function in real-life situations using more complex sentences and language structures. They will real material on familiar topics and produce short writing samples. </t>
+  </si>
+  <si>
+    <t>Students continue to develop their skills in listening, speaking, reading, and writing, while learning how to use more complex language structures on more abstract concepts. The themes of the class include Rights and Responsibilities, Future Plans and Choices, Teen Culture, Environment, and Humanities.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students learn basic language structure and pronunciation in order to read simple Latin passages. The relationship of English to Latin is emphasized in vocabulary, word derivation, and meanings of prefixes and suffixes. Students also learn about the geography, history, government, and culture of the Roman Empire. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students learn more vocabulary, more complex language structures and syntax so that they are able to read more challenging passages in Latin. Students continue to study Roman life and Rome’s contribution to our civilization. </t>
+  </si>
+  <si>
+    <t>Students develop and refine their reading skills, learn additional vocabulary, and learn more complex language structures and syntax. Through translation and interpretation, students gain a greater understanding of the foundation of Western government and civilization.</t>
+  </si>
+  <si>
+    <t>Topics include linear equations and inequalities, systems of linear equations, relations, functions, polynomials, and statistics. Emphasis is placed on making connections in algebra to geometry and statistics.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This class goes beyond the scope of Algebra I. Students are expected to master algebraic mechanics and understand the underlying theory, as well as apply the concepts to real-world situations. Emphasis is placed on algebraic connections to arithmetic, geometry, and statistics. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This course emphasizes two- and three-dimensional reasoning skills, coordinate and transformational geometry, and the use of geometric models to solve problems. </t>
+  </si>
+  <si>
+    <t>Goes beyond the scope of Geometry. Heavily uses proofs to verify theorems. Students investigate non-Euclidean geometries and formal logic.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topics include function, polynomials, rational expressions, complex numbers, exponential and logarithmic equations, arithmetic and geometric sequences and series, and data analysis. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students are expected to not only master algebraic mechanics but also to understand the underlying theory and to apply concepts to real-world situations in a meaningful way. Additional topics include matrices, infinite geometric sequences and series, permutations and combinations, and selected topics in discrete math. Emphasis is on modeling, logic, and interpretation of related graphs. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students learn how to code in Java, developing their skills in defining, writing, and running programs on a computer. Students will work with both mathematical and non-mathematical problems. </t>
   </si>
 </sst>
 </file>
@@ -511,13 +556,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -801,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -896,322 +944,391 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D37" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>77</v>
       </c>

</xml_diff>

<commit_message>
Update Courses pt. 2
/title
</commit_message>
<xml_diff>
--- a/Course Description Sample Sheet.xlsx
+++ b/Course Description Sample Sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="177">
   <si>
     <t>English 9</t>
   </si>
@@ -537,6 +537,24 @@
   </si>
   <si>
     <t>In comparison to World History and Geography 1, students will investigate some topics at a deeper level. Students are encouraged to think independently while developing group process skills.</t>
+  </si>
+  <si>
+    <t>In Journalism 1 students learn the history and language of journalism; develop communication skills in writing, designing and editing for a variety of media; understand news and the process of publication; and become more critical readers and viewers of mass media.</t>
+  </si>
+  <si>
+    <t>In Photojournalism 1, students learn the principles of interviewing, copywriting, photography, layout, and design. Students will use publishing software to create pages for the school's yearbook. This course requires some after school time. This course requires an application and approval by instructor.</t>
+  </si>
+  <si>
+    <t>This course provides students an opportunity for additional writing instruction beyond the standard English program. Experimentation with many forms of writing is encouraged, with an emphasis on poetry, short stories, plays, and all forms of descriptive writing.</t>
+  </si>
+  <si>
+    <t>This course involves the study of classic and award-winning films. Students critique both the artistic and technical merits of the films. Students will produce short films each semester.</t>
+  </si>
+  <si>
+    <t>Students will research the current topics and write cases both affirming and negating the resolutions. Students will also take part in regular in-class mock debates. This class can be used as preparation time for participation in the Woodson Debate team. Participation in at least one evening or Saturday debate event is required.</t>
+  </si>
+  <si>
+    <t>Students will be familiarized with some of the major forensic events, including Original Oratory, Dramatic Interpretation, Impromptu speaking, and Extemporaneous speaking. This class can be used as prep time for participation in the WTW Forensics (Speech) team. Participation in at least one evening or Saturday event is required.</t>
   </si>
 </sst>
 </file>
@@ -888,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1242,6 +1260,9 @@
       <c r="A50" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="D50" s="5" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
@@ -1252,16 +1273,25 @@
       <c r="A52" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="D52" s="5" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="D53" s="5" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="D54" s="5" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
@@ -1272,10 +1302,16 @@
       <c r="A56" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="D56" s="5" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>54</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added more course descriptions
/title
</commit_message>
<xml_diff>
--- a/Course Description Sample Sheet.xlsx
+++ b/Course Description Sample Sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="189">
   <si>
     <t>English 9</t>
   </si>
@@ -555,6 +555,42 @@
   </si>
   <si>
     <t>Students will be familiarized with some of the major forensic events, including Original Oratory, Dramatic Interpretation, Impromptu speaking, and Extemporaneous speaking. This class can be used as prep time for participation in the WTW Forensics (Speech) team. Participation in at least one evening or Saturday event is required.</t>
+  </si>
+  <si>
+    <t>This is an adapted curriculum elective geared to students needing intensive support. Instruction is very concrete with extensive physical modeling and assistance. The course will identify work-related abilities, provide training and work skills, and prepare students for post-secondary participation in community-based worksites.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This course is designed to support instruction in the science content area; does not require SOL testing. Instruction is individualized based on needs identified in the IEP to help students gain a basic content vocabulary, knowledge and skills and designed to be taught at the learning pace of the individual students. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This course is designed to support instruction in the English content area; does not require SOL testing. Instruction is individualized based on needs identified in the IEP to help students gain a basic content vocabulary, knowledge and skills and designed to be taught at the learning pace of the individual students. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students develop the ability to communicate about themselves and their immediate environment using simple sentences containing basic language structures. This communication is evidenced in signing, receiving signs and non-manual gestures, and reading. Students begin to explore and study the themes of Personal and Family Life, School Life, Social Life, and Community Life. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students continue to develop proficiency in American Sign Language. They learn to function in real-life situations using more complex language structures and a wider range of vocabulary. Students continue to explore as they study the themes of Home Life, Student Life, Leisure Time, and Vacation and Travel. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students continue to develop and refine their proficiency in American Sign Language. They communicate using more complex language structures on a variety of topics, moving from concrete to more abstract concepts. Students gain a deeper understanding of the world around them while studying Rights and Responsibilities, Future Plans and Choices, Teen Culture, Environment, and Humanities. </t>
+  </si>
+  <si>
+    <t>Foundations of World History/Geography is a one-credit elective course designed to support in the World History content area; does not require SOL testing. Instruction is individualized based on needs identified in the IEP to help students gain a basic content vocabulary, knowledge and skills and designed to be taught at the learning pace of the individual students.</t>
+  </si>
+  <si>
+    <t>This comprehensive individualized program is designed to prepare students for a style of living that will require a minimum of dependence on family. The course is geared to meet the needs of the students as they prepare to enter employment and emphasizes developing interpersonal skills, following directions, working independently, completing a task, and developing self-advocacy and other community living skills.</t>
+  </si>
+  <si>
+    <t>This course, offered at Davis and Pulley Centers and STEP, is designed to teach students with disabilities skills for independent living.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explore a variety of exciting opportunities and materials to inform the artmaking process. Learn to think conceptually and realize potential as a creative and critical thinker in order to meet the challenges of 21st century living. Explore personal interests while developing skills in the areas of drawing, painting, printmaking, ceramics, sculpture, and digital media. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theatre Arts 1 provides students with a survey of the theatre arts, allowing student’s opportunities to experience and appreciate dramatic literature, and participate in the creative processes of performance and production. This course emphasizes skill development and provides theatrical opportunities that enable students to determine personal areas of interest. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students are provided the opportunity to sample a variety of musical experiences in a non-performing music class. Course content includes beginning guitar and class piano experience, as well as various modules designed to assist students in developing music reading and composing skills. </t>
   </si>
 </sst>
 </file>
@@ -906,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="M144" sqref="M144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1145,21 +1181,33 @@
       <c r="A30" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="D30" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="D31" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="D32" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="D33" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
@@ -1197,26 +1245,41 @@
       <c r="A38" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="D38" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="D39" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>37</v>
       </c>
+      <c r="D40" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="D41" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="D42" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
@@ -1652,159 +1715,213 @@
         <v>109</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D126" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D127" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D128" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D129" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D130" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D131" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D132" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D133" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D134" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D135" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D136" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D137" s="7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D138" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D139" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D140" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D141" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D142" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>140</v>
+      </c>
+      <c r="D143" s="7" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>